<commit_message>
Updated UserManualReview.xls with BTA's comments
Signed-off-by: alfredoh1234 <alfredo.herrera@ieee.org>
</commit_message>
<xml_diff>
--- a/cores/cv32e40p/UserManualReview.xlsx
+++ b/cores/cv32e40p/UserManualReview.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arbink\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aherrera\workspace\core-v-docs\cores\cv32e40p\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE93889D-52C3-444C-9190-89545E0B68DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A331777A-46F2-4347-B154-56C3A303307A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28845" yWindow="465" windowWidth="24645" windowHeight="15075" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Review" sheetId="1" r:id="rId1"/>
     <sheet name="DO NOT DELETE" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Review!$B$2:$F$82</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="137">
   <si>
     <t>Major Section</t>
   </si>
@@ -438,6 +441,162 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Missing chapter numbers in Table of Contents
+Figure 1 missing debug interface and interrupts</t>
+  </si>
+  <si>
+    <t>Missing links to other sections
+Missing PULP specific extensions:
+   * Bit manipulation
+Incomplete PULP specific extensions:
+   * ALU extensions:
+     * bit manipulation
+     * general-ALU 
+     * immediate branching 
+Included but not supported PULP specific extensions:
+   * Multiply-Accumulate extensions</t>
+  </si>
+  <si>
+    <t>Not found on Read-the-Docs</t>
+  </si>
+  <si>
+    <t>Not linked to repository profile, which makes it less useful</t>
+  </si>
+  <si>
+    <t>Not found on Read-the-Docs, but it was in original document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HWLoop constraints </t>
+  </si>
+  <si>
+    <t>The HWLoop constraints section is not sufficiently defined.
+It seems clear it needs to be verified, but difficult from current info in User Manual</t>
+  </si>
+  <si>
+    <t>CSR table</t>
+  </si>
+  <si>
+    <t>Read the Docs "Control and Status Registers" table has errors (Issue #76)</t>
+  </si>
+  <si>
+    <t>DCSR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The following fields are available in the Debugger-CSR when in debugger mode. fields with (*) are different from Privileged ISA document and missing in user manual:
+|------------------------------------------------------------|
+|Address| R/W  |               Description                           |
+|----------|-------|----------------------------------------|
+| [31:28]  |    R     | Ext. debug support exists             |
+|       [15]  | R/W  | ebreakm                                              |
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|       [13]  | R/W  | ebreaks (*)                                        |
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|       [12]  | R/W  | ebreaku                                               |
+|       [11]  |WARL| stepi                                                     |
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|       [10]  |WARL| stopcount (*)                                    |
+|         [9]  |WARL| stoptime (*)                                      |
+|      [8:6]  |    R     | cause (*)                                             |
+|         [4]  |R/W| mprven (*)                                            |
+|         [3]  |R/W| nmip (*)                                                  |
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>|          [2] |R/W| step                                                           |
+|      [1:0]  |   R   | returns current priviledge mode  |
+|------------------------------------------------------------|</t>
+    </r>
+  </si>
+  <si>
+    <t>See verification plan:
+https://github.com/openhwgroup/core-v-docs/blob/master/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-hwloop.xlsx</t>
+  </si>
+  <si>
+    <t>Core Halt controlled from Debug Module, not in User Document. Missing block diagram. See verification plan:
+https://github.com/openhwgroup/core-v-docs/blob/master/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-hwloop.xlsx</t>
+  </si>
+  <si>
+    <t>See verification plan:
+https://github.com/openhwgroup/core-v-docs/blob/master/verif/CV32E40P/VerificationPlan/xpulp_instruction_extensions/CV32E40P_xpulp-postinc-loadstore.xlsx</t>
+  </si>
+  <si>
+    <t>Split into three section</t>
+  </si>
+  <si>
+    <t>ALU - bit manipulation</t>
+  </si>
+  <si>
+    <t>Clarify [github issue #5] Bit Manipulation: what happens when indexes are out-of-bounds? https://github.com/openhwgroup/core-v-docs/issues/5</t>
+  </si>
+  <si>
+    <t>ALU - general ALU</t>
+  </si>
+  <si>
+    <t>ALU - immediate branch</t>
+  </si>
+  <si>
+    <t>related to [githib issue #213]
+RI5CY: User Manual v4.2: p.clip* instructions imply ls2 unsigned rs1 signed for all
+Requested that a sentence be added to the document between the header of section 14 and the first subsection 14.1 saying:  "All numbers are signed, unless specifically indicated."</t>
+  </si>
+  <si>
+    <t>[githib issue #214]
+RI5CY: User Manual v4.2: p.clipr instructions opcode seems wrong
+It was requested that a sentence be added to the document between the header of section 14 and the first subsection 14.1 saying: "For numbers that are not 32-bit, sign-extension (Sext) is specified; but this is not the case for Gen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+[github issue #220]
+Typo: RI5CY User Manual v4.2, description of p.addN, p.adduN 
+shouldn't the value of the right-shift be 2^(ls3-1) to divide by 2 when ls3 = 2 ?</t>
+  </si>
+  <si>
+    <t>As far as I know, this was never in-scope</t>
+  </si>
+  <si>
+    <t>Issue#233 RI5CY: User Manual v4.2-14.5.1 Vectorial ALU Operations table missing information: https://github.com/openhwgroup/cv32e40p/issues/233</t>
+  </si>
+  <si>
+    <t>Issue#236
+RI5CY: User Manual v4.2-14.5.1 pv.*.div2, pv.*.div4 and pv.*.div8 unclear</t>
+  </si>
+  <si>
+    <t>issue#240: RI5CY: User Manual v4.2-14.5.1 error in complex imaginary multiplication pv.cplxmul.i.*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">issue#241:
+RI5CY: User Manual v4.2-14.5.1 missing information for pv.shuffle2.* instruction </t>
   </si>
 </sst>
 </file>
@@ -475,7 +634,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -486,6 +645,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDEE7E5"/>
         <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,8 +730,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,31 +1150,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F528"/>
+  <dimension ref="B1:F545"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
     <col min="5" max="5" width="81" customWidth="1"/>
     <col min="6" max="6" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -991,18 +1191,20 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="14"/>
       <c r="C4" t="s">
         <v>5</v>
@@ -1015,7 +1217,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" t="s">
         <v>7</v>
@@ -1030,2371 +1232,2617 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="132" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
       <c r="F7" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="14"/>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E14" s="5"/>
       <c r="F14" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="14"/>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="F15" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
+      <c r="E16" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="14"/>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="8" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="14"/>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="E18" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
       <c r="D19" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
+      <c r="C22" t="s">
+        <v>29</v>
+      </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="14"/>
-      <c r="D23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>39</v>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="14"/>
-      <c r="D24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="14"/>
-      <c r="C25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>42</v>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>34</v>
+    <row r="26" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
-      <c r="C27" t="s">
-        <v>44</v>
-      </c>
       <c r="D27" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="14"/>
-      <c r="C28" t="s">
-        <v>41</v>
-      </c>
       <c r="D28" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F28" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="14"/>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="14"/>
-      <c r="C30" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="10" t="s">
-        <v>50</v>
+      <c r="E30" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B31" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7" t="s">
-        <v>52</v>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+      <c r="D31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>54</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="14"/>
+      <c r="C32" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="F33" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="52.8" x14ac:dyDescent="0.25">
       <c r="B34" s="14"/>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="14"/>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E35" s="5"/>
       <c r="F35" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="14"/>
-      <c r="C36" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>61</v>
+      <c r="C36" t="s">
+        <v>46</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="B37" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="14"/>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="14"/>
       <c r="C38" s="9" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B39" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="14"/>
-      <c r="D40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B39" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E40" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="14"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9" t="s">
+      <c r="E40" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B42" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="14"/>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="14"/>
-      <c r="D43" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E43" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="14"/>
-      <c r="D44" s="4" t="s">
+      <c r="C44" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F44" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="14"/>
-      <c r="D45" s="4" t="s">
+      <c r="E45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E45" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B46" s="14"/>
-      <c r="C46" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E46" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="14"/>
       <c r="C47" s="9" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
       <c r="E47" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B48" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B49" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="14"/>
+      <c r="D49" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F49" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="B50" s="15"/>
+      <c r="E49" s="26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="14"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F50" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="3"/>
+      <c r="D51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="F51" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="14"/>
-      <c r="C52" t="s">
-        <v>86</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B53" s="14"/>
-      <c r="C53" t="s">
-        <v>88</v>
-      </c>
       <c r="D53" s="4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="F53" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="14"/>
-      <c r="C54" t="s">
-        <v>90</v>
-      </c>
       <c r="D54" s="4" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F54" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="14"/>
-      <c r="C55" s="9"/>
-      <c r="D55" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="10" t="s">
-        <v>92</v>
-      </c>
+      <c r="C55" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="5"/>
       <c r="F55" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B56" s="6" t="s">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+      <c r="C56" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E57" s="29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="20"/>
+      <c r="C58" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E58" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="237.6" x14ac:dyDescent="0.25">
+      <c r="B59" s="17"/>
+      <c r="C59" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B60" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F60" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B61" s="15"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="F61" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="3"/>
+      <c r="F62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B63" s="21"/>
+      <c r="C63" t="s">
+        <v>86</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="21"/>
+      <c r="C64" t="s">
+        <v>88</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B65" s="21"/>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="22"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C56" s="6"/>
-      <c r="D56" s="6" t="s">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E67" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F56" s="13" t="s">
+      <c r="F67" s="13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="16" t="s">
+    <row r="68" spans="2:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="3" t="s">
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F69" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="16"/>
-      <c r="C58" t="s">
+    <row r="70" spans="2:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B70" s="21"/>
+      <c r="C70" t="s">
         <v>49</v>
       </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="13" t="s">
+      <c r="D70" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F70" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="16"/>
-      <c r="C59" t="s">
+    <row r="71" spans="2:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B71" s="21"/>
+      <c r="C71" t="s">
         <v>97</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="13" t="s">
+      <c r="D71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F71" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B60" s="16"/>
-      <c r="C60" t="s">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="21"/>
+      <c r="C72" t="s">
         <v>98</v>
       </c>
-      <c r="D60" s="4"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="13" t="s">
+      <c r="D72" s="4"/>
+      <c r="E72" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F72" s="13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="16"/>
-      <c r="C61" t="s">
-        <v>51</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B62" s="16"/>
-      <c r="C62" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" s="9"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D63" s="4"/>
-      <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D64" s="4"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D65" s="4"/>
-      <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D66" s="4"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D67" s="4"/>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D68" s="4"/>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D69" s="4"/>
-      <c r="E69" s="5"/>
-    </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D70" s="4"/>
-      <c r="E70" s="5"/>
-    </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D71" s="4"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D72" s="4"/>
-      <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B73" s="21"/>
+      <c r="C73" t="s">
+        <v>125</v>
+      </c>
       <c r="D73" s="4"/>
-      <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D74" s="4"/>
-      <c r="E74" s="5"/>
-    </row>
-    <row r="75" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D75" s="4"/>
-      <c r="E75" s="5"/>
-    </row>
-    <row r="76" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D76" s="4"/>
-      <c r="E76" s="5"/>
-    </row>
-    <row r="77" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E73" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F73" s="13"/>
+    </row>
+    <row r="74" spans="2:6" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="B74" s="21"/>
+      <c r="C74" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E74" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="F74" s="13"/>
+    </row>
+    <row r="75" spans="2:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="B75" s="21"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E75" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="13"/>
+    </row>
+    <row r="76" spans="2:6" ht="66" x14ac:dyDescent="0.25">
+      <c r="B76" s="21"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F76" s="13"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="21"/>
+      <c r="C77" t="s">
+        <v>128</v>
+      </c>
       <c r="D77" s="4"/>
       <c r="E77" s="5"/>
-    </row>
-    <row r="78" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D78" s="4"/>
-      <c r="E78" s="5"/>
-    </row>
-    <row r="79" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D79" s="4"/>
-      <c r="E79" s="5"/>
-    </row>
-    <row r="80" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D80" s="4"/>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D81" s="4"/>
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D82" s="4"/>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="13"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="21"/>
+      <c r="C78" t="s">
+        <v>51</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F78" s="13"/>
+    </row>
+    <row r="79" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B79" s="21"/>
+      <c r="C79" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F79" s="13"/>
+    </row>
+    <row r="80" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B80" s="21"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B81" s="21"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B82" s="21"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D83" s="4"/>
       <c r="E83" s="5"/>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D84" s="4"/>
       <c r="E84" s="5"/>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D85" s="4"/>
       <c r="E85" s="5"/>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D86" s="4"/>
       <c r="E86" s="5"/>
     </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D87" s="4"/>
       <c r="E87" s="5"/>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D88" s="4"/>
       <c r="E88" s="5"/>
     </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D89" s="4"/>
       <c r="E89" s="5"/>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D90" s="4"/>
       <c r="E90" s="5"/>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D91" s="4"/>
       <c r="E91" s="5"/>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D92" s="4"/>
       <c r="E92" s="5"/>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D93" s="4"/>
       <c r="E93" s="5"/>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D94" s="4"/>
       <c r="E94" s="5"/>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D95" s="4"/>
       <c r="E95" s="5"/>
     </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D96" s="4"/>
       <c r="E96" s="5"/>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D97" s="4"/>
       <c r="E97" s="5"/>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D98" s="4"/>
       <c r="E98" s="5"/>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D99" s="4"/>
       <c r="E99" s="5"/>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D100" s="4"/>
       <c r="E100" s="5"/>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D101" s="4"/>
       <c r="E101" s="5"/>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D102" s="4"/>
       <c r="E102" s="5"/>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D103" s="4"/>
       <c r="E103" s="5"/>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D104" s="4"/>
       <c r="E104" s="5"/>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D105" s="4"/>
       <c r="E105" s="5"/>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D106" s="4"/>
       <c r="E106" s="5"/>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D107" s="4"/>
       <c r="E107" s="5"/>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D108" s="4"/>
       <c r="E108" s="5"/>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D109" s="4"/>
       <c r="E109" s="5"/>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D110" s="4"/>
       <c r="E110" s="5"/>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D111" s="4"/>
       <c r="E111" s="5"/>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D112" s="4"/>
       <c r="E112" s="5"/>
     </row>
-    <row r="113" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D113" s="4"/>
       <c r="E113" s="5"/>
     </row>
-    <row r="114" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D114" s="4"/>
       <c r="E114" s="5"/>
     </row>
-    <row r="115" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D115" s="4"/>
       <c r="E115" s="5"/>
     </row>
-    <row r="116" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D116" s="4"/>
       <c r="E116" s="5"/>
     </row>
-    <row r="117" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D117" s="4"/>
       <c r="E117" s="5"/>
     </row>
-    <row r="118" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D118" s="4"/>
       <c r="E118" s="5"/>
     </row>
-    <row r="119" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D119" s="4"/>
       <c r="E119" s="5"/>
     </row>
-    <row r="120" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D120" s="4"/>
       <c r="E120" s="5"/>
     </row>
-    <row r="121" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D121" s="4"/>
       <c r="E121" s="5"/>
     </row>
-    <row r="122" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D122" s="4"/>
       <c r="E122" s="5"/>
     </row>
-    <row r="123" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D123" s="4"/>
       <c r="E123" s="5"/>
     </row>
-    <row r="124" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D124" s="4"/>
       <c r="E124" s="5"/>
     </row>
-    <row r="125" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D125" s="4"/>
       <c r="E125" s="5"/>
     </row>
-    <row r="126" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D126" s="4"/>
       <c r="E126" s="5"/>
     </row>
-    <row r="127" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D127" s="4"/>
       <c r="E127" s="5"/>
     </row>
-    <row r="128" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D128" s="4"/>
       <c r="E128" s="5"/>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D129" s="4"/>
       <c r="E129" s="5"/>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D130" s="4"/>
       <c r="E130" s="5"/>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D131" s="4"/>
       <c r="E131" s="5"/>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D132" s="4"/>
       <c r="E132" s="5"/>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D133" s="4"/>
       <c r="E133" s="5"/>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D134" s="4"/>
       <c r="E134" s="5"/>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D135" s="4"/>
       <c r="E135" s="5"/>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D136" s="4"/>
       <c r="E136" s="5"/>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D137" s="4"/>
       <c r="E137" s="5"/>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D138" s="4"/>
       <c r="E138" s="5"/>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D139" s="4"/>
       <c r="E139" s="5"/>
     </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D140" s="4"/>
       <c r="E140" s="5"/>
     </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D141" s="4"/>
       <c r="E141" s="5"/>
     </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D142" s="4"/>
       <c r="E142" s="5"/>
     </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D143" s="4"/>
       <c r="E143" s="5"/>
     </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D144" s="4"/>
       <c r="E144" s="5"/>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D145" s="4"/>
       <c r="E145" s="5"/>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D146" s="4"/>
       <c r="E146" s="5"/>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D147" s="4"/>
       <c r="E147" s="5"/>
     </row>
-    <row r="148" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D148" s="4"/>
       <c r="E148" s="5"/>
     </row>
-    <row r="149" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D149" s="4"/>
       <c r="E149" s="5"/>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D150" s="4"/>
       <c r="E150" s="5"/>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D151" s="4"/>
       <c r="E151" s="5"/>
     </row>
-    <row r="152" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D152" s="4"/>
       <c r="E152" s="5"/>
     </row>
-    <row r="153" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D153" s="4"/>
       <c r="E153" s="5"/>
     </row>
-    <row r="154" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D154" s="4"/>
       <c r="E154" s="5"/>
     </row>
-    <row r="155" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D155" s="4"/>
       <c r="E155" s="5"/>
     </row>
-    <row r="156" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D156" s="4"/>
       <c r="E156" s="5"/>
     </row>
-    <row r="157" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D157" s="4"/>
       <c r="E157" s="5"/>
     </row>
-    <row r="158" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D158" s="4"/>
       <c r="E158" s="5"/>
     </row>
-    <row r="159" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D159" s="4"/>
       <c r="E159" s="5"/>
     </row>
-    <row r="160" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D160" s="4"/>
       <c r="E160" s="5"/>
     </row>
-    <row r="161" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D161" s="4"/>
       <c r="E161" s="5"/>
     </row>
-    <row r="162" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D162" s="4"/>
       <c r="E162" s="5"/>
     </row>
-    <row r="163" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D163" s="4"/>
       <c r="E163" s="5"/>
     </row>
-    <row r="164" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D164" s="4"/>
       <c r="E164" s="5"/>
     </row>
-    <row r="165" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D165" s="4"/>
       <c r="E165" s="5"/>
     </row>
-    <row r="166" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D166" s="4"/>
       <c r="E166" s="5"/>
     </row>
-    <row r="167" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D167" s="4"/>
       <c r="E167" s="5"/>
     </row>
-    <row r="168" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D168" s="4"/>
       <c r="E168" s="5"/>
     </row>
-    <row r="169" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D169" s="4"/>
       <c r="E169" s="5"/>
     </row>
-    <row r="170" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D170" s="4"/>
       <c r="E170" s="5"/>
     </row>
-    <row r="171" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D171" s="4"/>
       <c r="E171" s="5"/>
     </row>
-    <row r="172" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D172" s="4"/>
       <c r="E172" s="5"/>
     </row>
-    <row r="173" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D173" s="4"/>
       <c r="E173" s="5"/>
     </row>
-    <row r="174" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D174" s="4"/>
       <c r="E174" s="5"/>
     </row>
-    <row r="175" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D175" s="4"/>
       <c r="E175" s="5"/>
     </row>
-    <row r="176" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D176" s="4"/>
       <c r="E176" s="5"/>
     </row>
-    <row r="177" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D177" s="4"/>
       <c r="E177" s="5"/>
     </row>
-    <row r="178" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D178" s="4"/>
       <c r="E178" s="5"/>
     </row>
-    <row r="179" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D179" s="4"/>
       <c r="E179" s="5"/>
     </row>
-    <row r="180" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D180" s="4"/>
       <c r="E180" s="5"/>
     </row>
-    <row r="181" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D181" s="4"/>
       <c r="E181" s="5"/>
     </row>
-    <row r="182" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D182" s="4"/>
       <c r="E182" s="5"/>
     </row>
-    <row r="183" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D183" s="4"/>
       <c r="E183" s="5"/>
     </row>
-    <row r="184" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D184" s="4"/>
       <c r="E184" s="5"/>
     </row>
-    <row r="185" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D185" s="4"/>
       <c r="E185" s="5"/>
     </row>
-    <row r="186" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D186" s="4"/>
       <c r="E186" s="5"/>
     </row>
-    <row r="187" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D187" s="4"/>
       <c r="E187" s="5"/>
     </row>
-    <row r="188" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D188" s="4"/>
       <c r="E188" s="5"/>
     </row>
-    <row r="189" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D189" s="4"/>
       <c r="E189" s="5"/>
     </row>
-    <row r="190" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D190" s="4"/>
       <c r="E190" s="5"/>
     </row>
-    <row r="191" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D191" s="4"/>
       <c r="E191" s="5"/>
     </row>
-    <row r="192" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D192" s="4"/>
       <c r="E192" s="5"/>
     </row>
-    <row r="193" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D193" s="4"/>
       <c r="E193" s="5"/>
     </row>
-    <row r="194" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D194" s="4"/>
       <c r="E194" s="5"/>
     </row>
-    <row r="195" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D195" s="4"/>
       <c r="E195" s="5"/>
     </row>
-    <row r="196" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D196" s="4"/>
       <c r="E196" s="5"/>
     </row>
-    <row r="197" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D197" s="4"/>
       <c r="E197" s="5"/>
     </row>
-    <row r="198" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D198" s="4"/>
       <c r="E198" s="5"/>
     </row>
-    <row r="199" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D199" s="4"/>
       <c r="E199" s="5"/>
     </row>
-    <row r="200" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D200" s="4"/>
       <c r="E200" s="5"/>
     </row>
-    <row r="201" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D201" s="4"/>
       <c r="E201" s="5"/>
     </row>
-    <row r="202" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D202" s="4"/>
       <c r="E202" s="5"/>
     </row>
-    <row r="203" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D203" s="4"/>
       <c r="E203" s="5"/>
     </row>
-    <row r="204" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D204" s="4"/>
       <c r="E204" s="5"/>
     </row>
-    <row r="205" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D205" s="4"/>
       <c r="E205" s="5"/>
     </row>
-    <row r="206" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D206" s="4"/>
       <c r="E206" s="5"/>
     </row>
-    <row r="207" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D207" s="4"/>
       <c r="E207" s="5"/>
     </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D208" s="4"/>
       <c r="E208" s="5"/>
     </row>
-    <row r="209" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D209" s="4"/>
       <c r="E209" s="5"/>
     </row>
-    <row r="210" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D210" s="4"/>
       <c r="E210" s="5"/>
     </row>
-    <row r="211" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D211" s="4"/>
       <c r="E211" s="5"/>
     </row>
-    <row r="212" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D212" s="4"/>
       <c r="E212" s="5"/>
     </row>
-    <row r="213" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D213" s="4"/>
       <c r="E213" s="5"/>
     </row>
-    <row r="214" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D214" s="4"/>
       <c r="E214" s="5"/>
     </row>
-    <row r="215" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D215" s="4"/>
       <c r="E215" s="5"/>
     </row>
-    <row r="216" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D216" s="4"/>
       <c r="E216" s="5"/>
     </row>
-    <row r="217" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D217" s="4"/>
       <c r="E217" s="5"/>
     </row>
-    <row r="218" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D218" s="4"/>
       <c r="E218" s="5"/>
     </row>
-    <row r="219" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D219" s="4"/>
       <c r="E219" s="5"/>
     </row>
-    <row r="220" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D220" s="4"/>
       <c r="E220" s="5"/>
     </row>
-    <row r="221" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D221" s="4"/>
       <c r="E221" s="5"/>
     </row>
-    <row r="222" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D222" s="4"/>
       <c r="E222" s="5"/>
     </row>
-    <row r="223" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D223" s="4"/>
       <c r="E223" s="5"/>
     </row>
-    <row r="224" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D224" s="4"/>
       <c r="E224" s="5"/>
     </row>
-    <row r="225" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D225" s="4"/>
       <c r="E225" s="5"/>
     </row>
-    <row r="226" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D226" s="4"/>
       <c r="E226" s="5"/>
     </row>
-    <row r="227" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D227" s="4"/>
       <c r="E227" s="5"/>
     </row>
-    <row r="228" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D228" s="4"/>
       <c r="E228" s="5"/>
     </row>
-    <row r="229" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D229" s="4"/>
       <c r="E229" s="5"/>
     </row>
-    <row r="230" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D230" s="4"/>
       <c r="E230" s="5"/>
     </row>
-    <row r="231" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D231" s="4"/>
       <c r="E231" s="5"/>
     </row>
-    <row r="232" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D232" s="4"/>
       <c r="E232" s="5"/>
     </row>
-    <row r="233" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D233" s="4"/>
       <c r="E233" s="5"/>
     </row>
-    <row r="234" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D234" s="4"/>
       <c r="E234" s="5"/>
     </row>
-    <row r="235" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D235" s="4"/>
       <c r="E235" s="5"/>
     </row>
-    <row r="236" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D236" s="4"/>
       <c r="E236" s="5"/>
     </row>
-    <row r="237" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D237" s="4"/>
       <c r="E237" s="5"/>
     </row>
-    <row r="238" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D238" s="4"/>
       <c r="E238" s="5"/>
     </row>
-    <row r="239" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D239" s="4"/>
       <c r="E239" s="5"/>
     </row>
-    <row r="240" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D240" s="4"/>
       <c r="E240" s="5"/>
     </row>
-    <row r="241" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D241" s="4"/>
       <c r="E241" s="5"/>
     </row>
-    <row r="242" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D242" s="4"/>
       <c r="E242" s="5"/>
     </row>
-    <row r="243" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D243" s="4"/>
       <c r="E243" s="5"/>
     </row>
-    <row r="244" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D244" s="4"/>
       <c r="E244" s="5"/>
     </row>
-    <row r="245" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D245" s="4"/>
       <c r="E245" s="5"/>
     </row>
-    <row r="246" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D246" s="4"/>
       <c r="E246" s="5"/>
     </row>
-    <row r="247" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D247" s="4"/>
       <c r="E247" s="5"/>
     </row>
-    <row r="248" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D248" s="4"/>
       <c r="E248" s="5"/>
     </row>
-    <row r="249" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D249" s="4"/>
-    </row>
-    <row r="250" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E249" s="5"/>
+    </row>
+    <row r="250" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D250" s="4"/>
-    </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E250" s="5"/>
+    </row>
+    <row r="251" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D251" s="4"/>
-    </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E251" s="5"/>
+    </row>
+    <row r="252" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D252" s="4"/>
-    </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E252" s="5"/>
+    </row>
+    <row r="253" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D253" s="4"/>
-    </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E253" s="5"/>
+    </row>
+    <row r="254" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D254" s="4"/>
-    </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E254" s="5"/>
+    </row>
+    <row r="255" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D255" s="4"/>
-    </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E255" s="5"/>
+    </row>
+    <row r="256" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D256" s="4"/>
-    </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E256" s="5"/>
+    </row>
+    <row r="257" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D257" s="4"/>
-    </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E257" s="5"/>
+    </row>
+    <row r="258" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D258" s="4"/>
-    </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E258" s="5"/>
+    </row>
+    <row r="259" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D259" s="4"/>
-    </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E259" s="5"/>
+    </row>
+    <row r="260" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D260" s="4"/>
-    </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E260" s="5"/>
+    </row>
+    <row r="261" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D261" s="4"/>
-    </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E261" s="5"/>
+    </row>
+    <row r="262" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D262" s="4"/>
-    </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E262" s="5"/>
+    </row>
+    <row r="263" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D263" s="4"/>
-    </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E263" s="5"/>
+    </row>
+    <row r="264" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D264" s="4"/>
-    </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E264" s="5"/>
+    </row>
+    <row r="265" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D265" s="4"/>
-    </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="E265" s="5"/>
+    </row>
+    <row r="266" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D266" s="4"/>
     </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D267" s="4"/>
     </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D268" s="4"/>
     </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D269" s="4"/>
     </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D270" s="4"/>
     </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D271" s="4"/>
     </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D272" s="4"/>
     </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D274" s="4"/>
     </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D275" s="4"/>
     </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D276" s="4"/>
     </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D277" s="4"/>
     </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D278" s="4"/>
     </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D279" s="4"/>
     </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D280" s="4"/>
     </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D281" s="4"/>
     </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D282" s="4"/>
     </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D284" s="4"/>
     </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D285" s="4"/>
     </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D286" s="4"/>
     </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D287" s="4"/>
     </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D288" s="4"/>
     </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D289" s="4"/>
     </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D290" s="4"/>
     </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D291" s="4"/>
     </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D292" s="4"/>
     </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D293" s="4"/>
     </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D294" s="4"/>
     </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D295" s="4"/>
     </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D296" s="4"/>
     </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D297" s="4"/>
     </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D298" s="4"/>
     </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D299" s="4"/>
     </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D300" s="4"/>
     </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D301" s="4"/>
     </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D302" s="4"/>
     </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D303" s="4"/>
     </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D304" s="4"/>
     </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D305" s="4"/>
     </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D306" s="4"/>
     </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D307" s="4"/>
     </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D308" s="4"/>
     </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D309" s="4"/>
     </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D310" s="4"/>
     </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D311" s="4"/>
     </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D312" s="4"/>
     </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D313" s="4"/>
     </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D314" s="4"/>
     </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D315" s="4"/>
     </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D316" s="4"/>
     </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D317" s="4"/>
     </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D318" s="4"/>
     </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D319" s="4"/>
     </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D320" s="4"/>
     </row>
-    <row r="321" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D321" s="4"/>
     </row>
-    <row r="322" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D322" s="4"/>
     </row>
-    <row r="323" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D323" s="4"/>
     </row>
-    <row r="324" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D324" s="4"/>
     </row>
-    <row r="325" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D325" s="4"/>
     </row>
-    <row r="326" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D326" s="4"/>
     </row>
-    <row r="327" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D327" s="4"/>
     </row>
-    <row r="328" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D328" s="4"/>
     </row>
-    <row r="329" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D329" s="4"/>
     </row>
-    <row r="330" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D330" s="4"/>
     </row>
-    <row r="331" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D331" s="4"/>
     </row>
-    <row r="332" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D332" s="4"/>
     </row>
-    <row r="333" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D333" s="4"/>
     </row>
-    <row r="334" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D334" s="4"/>
     </row>
-    <row r="335" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D335" s="4"/>
     </row>
-    <row r="336" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D336" s="4"/>
     </row>
-    <row r="337" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D337" s="4"/>
     </row>
-    <row r="338" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D338" s="4"/>
     </row>
-    <row r="339" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D339" s="4"/>
     </row>
-    <row r="340" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D340" s="4"/>
     </row>
-    <row r="341" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D341" s="4"/>
     </row>
-    <row r="342" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D342" s="4"/>
     </row>
-    <row r="343" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D343" s="4"/>
     </row>
-    <row r="344" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D344" s="4"/>
     </row>
-    <row r="345" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D345" s="4"/>
     </row>
-    <row r="346" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D346" s="4"/>
     </row>
-    <row r="347" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D347" s="4"/>
     </row>
-    <row r="348" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D348" s="4"/>
     </row>
-    <row r="349" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D349" s="4"/>
     </row>
-    <row r="350" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D350" s="4"/>
     </row>
-    <row r="351" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D351" s="4"/>
     </row>
-    <row r="352" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D352" s="4"/>
     </row>
-    <row r="353" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D353" s="4"/>
     </row>
-    <row r="354" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D354" s="4"/>
     </row>
-    <row r="355" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D355" s="4"/>
     </row>
-    <row r="356" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D356" s="4"/>
     </row>
-    <row r="357" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D357" s="4"/>
     </row>
-    <row r="358" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D358" s="4"/>
     </row>
-    <row r="359" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D359" s="4"/>
     </row>
-    <row r="360" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D360" s="4"/>
     </row>
-    <row r="361" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D361" s="4"/>
     </row>
-    <row r="362" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D362" s="4"/>
     </row>
-    <row r="363" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D363" s="4"/>
     </row>
-    <row r="364" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D364" s="4"/>
     </row>
-    <row r="365" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D365" s="4"/>
     </row>
-    <row r="366" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D366" s="4"/>
     </row>
-    <row r="367" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D367" s="4"/>
     </row>
-    <row r="368" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D368" s="4"/>
     </row>
-    <row r="369" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D369" s="4"/>
     </row>
-    <row r="370" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D370" s="4"/>
     </row>
-    <row r="371" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D371" s="4"/>
     </row>
-    <row r="372" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D372" s="4"/>
     </row>
-    <row r="373" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D373" s="4"/>
     </row>
-    <row r="374" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D374" s="4"/>
     </row>
-    <row r="375" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D375" s="4"/>
     </row>
-    <row r="376" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D376" s="4"/>
     </row>
-    <row r="377" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D377" s="4"/>
     </row>
-    <row r="378" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D378" s="4"/>
     </row>
-    <row r="379" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D379" s="4"/>
     </row>
-    <row r="380" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D380" s="4"/>
     </row>
-    <row r="381" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D381" s="4"/>
     </row>
-    <row r="382" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D382" s="4"/>
     </row>
-    <row r="383" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D383" s="4"/>
     </row>
-    <row r="384" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D384" s="4"/>
     </row>
-    <row r="385" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="4"/>
     </row>
-    <row r="386" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="4"/>
     </row>
-    <row r="387" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="4"/>
     </row>
-    <row r="388" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D388" s="4"/>
     </row>
-    <row r="389" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D389" s="4"/>
     </row>
-    <row r="390" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D390" s="4"/>
     </row>
-    <row r="391" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D391" s="4"/>
     </row>
-    <row r="392" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D392" s="4"/>
     </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D393" s="4"/>
     </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D394" s="4"/>
     </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D395" s="4"/>
     </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D396" s="4"/>
     </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D397" s="4"/>
     </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D398" s="4"/>
     </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D399" s="4"/>
     </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D400" s="4"/>
     </row>
-    <row r="401" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D401" s="4"/>
     </row>
-    <row r="402" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D402" s="4"/>
     </row>
-    <row r="403" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D403" s="4"/>
     </row>
-    <row r="404" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D404" s="4"/>
     </row>
-    <row r="405" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D405" s="4"/>
     </row>
-    <row r="406" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D406" s="4"/>
     </row>
-    <row r="407" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D407" s="4"/>
     </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D408" s="4"/>
     </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D409" s="4"/>
     </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D410" s="4"/>
     </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D411" s="4"/>
     </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D412" s="4"/>
     </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D413" s="4"/>
     </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D414" s="4"/>
     </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D415" s="4"/>
     </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D416" s="4"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D417" s="4"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D418" s="4"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D419" s="4"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D420" s="4"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D421" s="4"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D422" s="4"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D423" s="4"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D424" s="4"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D425" s="4"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D426" s="4"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="4"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="4"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="4"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="4"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="4"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D432" s="4"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D433" s="4"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D434" s="4"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D435" s="4"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D436" s="4"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D437" s="4"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D438" s="4"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D439" s="4"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D440" s="4"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D441" s="4"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D442" s="4"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="4"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D444" s="4"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D445" s="4"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D446" s="4"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D447" s="4"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D448" s="4"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D449" s="4"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D450" s="4"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D451" s="4"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D452" s="4"/>
     </row>
-    <row r="453" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="453" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D453" s="4"/>
     </row>
-    <row r="454" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="454" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D454" s="4"/>
     </row>
-    <row r="455" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="455" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D455" s="4"/>
     </row>
-    <row r="456" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="456" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D456" s="4"/>
     </row>
-    <row r="457" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="457" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D457" s="4"/>
     </row>
-    <row r="458" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="458" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D458" s="4"/>
     </row>
-    <row r="459" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="459" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D459" s="4"/>
     </row>
-    <row r="460" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="460" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D460" s="4"/>
     </row>
-    <row r="461" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="461" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D461" s="4"/>
     </row>
-    <row r="462" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="462" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D462" s="4"/>
     </row>
-    <row r="463" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="463" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D463" s="4"/>
     </row>
-    <row r="464" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="464" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D464" s="4"/>
     </row>
-    <row r="465" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="465" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D465" s="4"/>
     </row>
-    <row r="466" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="466" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D466" s="4"/>
     </row>
-    <row r="467" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="467" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D467" s="4"/>
     </row>
-    <row r="468" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="468" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D468" s="4"/>
     </row>
-    <row r="469" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="469" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D469" s="4"/>
     </row>
-    <row r="470" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="470" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D470" s="4"/>
     </row>
-    <row r="471" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="471" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D471" s="4"/>
     </row>
-    <row r="472" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="472" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D472" s="4"/>
     </row>
-    <row r="473" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="473" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D473" s="4"/>
     </row>
-    <row r="474" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="474" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D474" s="4"/>
     </row>
-    <row r="475" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="475" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D475" s="4"/>
     </row>
-    <row r="476" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="476" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D476" s="4"/>
     </row>
-    <row r="477" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="477" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D477" s="4"/>
     </row>
-    <row r="478" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="478" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D478" s="4"/>
     </row>
-    <row r="479" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="479" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D479" s="4"/>
     </row>
-    <row r="480" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="480" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D480" s="4"/>
     </row>
-    <row r="481" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="481" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D481" s="4"/>
     </row>
-    <row r="482" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="482" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D482" s="4"/>
     </row>
-    <row r="483" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="483" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D483" s="4"/>
     </row>
-    <row r="484" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="484" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D484" s="4"/>
     </row>
-    <row r="485" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="485" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D485" s="4"/>
     </row>
-    <row r="486" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="486" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D486" s="4"/>
     </row>
-    <row r="487" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="487" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D487" s="4"/>
     </row>
-    <row r="488" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="488" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D488" s="4"/>
     </row>
-    <row r="489" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="489" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D489" s="4"/>
     </row>
-    <row r="490" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="490" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D490" s="4"/>
     </row>
-    <row r="491" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="491" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D491" s="4"/>
     </row>
-    <row r="492" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="492" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D492" s="4"/>
     </row>
-    <row r="493" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="493" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D493" s="4"/>
     </row>
-    <row r="494" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="494" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D494" s="4"/>
     </row>
-    <row r="495" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="495" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D495" s="4"/>
     </row>
-    <row r="496" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="496" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D496" s="4"/>
     </row>
-    <row r="497" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="497" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D497" s="4"/>
     </row>
-    <row r="498" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="498" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D498" s="4"/>
     </row>
-    <row r="499" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="499" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D499" s="4"/>
     </row>
-    <row r="500" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="500" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D500" s="4"/>
     </row>
-    <row r="501" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="501" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D501" s="4"/>
     </row>
-    <row r="502" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="502" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D502" s="4"/>
     </row>
-    <row r="503" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="503" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D503" s="4"/>
     </row>
-    <row r="504" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="504" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D504" s="4"/>
     </row>
-    <row r="505" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="505" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D505" s="4"/>
     </row>
-    <row r="506" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="506" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D506" s="4"/>
     </row>
-    <row r="507" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="507" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D507" s="4"/>
     </row>
-    <row r="508" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="508" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D508" s="4"/>
     </row>
-    <row r="509" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="509" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D509" s="4"/>
     </row>
-    <row r="510" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="510" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D510" s="4"/>
     </row>
-    <row r="511" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="511" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D511" s="4"/>
     </row>
-    <row r="512" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="512" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D512" s="4"/>
     </row>
-    <row r="513" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="513" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D513" s="4"/>
     </row>
-    <row r="514" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="514" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D514" s="4"/>
     </row>
-    <row r="515" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="515" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D515" s="4"/>
     </row>
-    <row r="516" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="516" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D516" s="4"/>
     </row>
-    <row r="517" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="517" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D517" s="4"/>
     </row>
-    <row r="518" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="518" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D518" s="4"/>
     </row>
-    <row r="519" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="519" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D519" s="4"/>
     </row>
-    <row r="520" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="520" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D520" s="4"/>
     </row>
-    <row r="521" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="521" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D521" s="4"/>
     </row>
-    <row r="522" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="522" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D522" s="4"/>
     </row>
-    <row r="523" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="523" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D523" s="4"/>
     </row>
-    <row r="524" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="524" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D524" s="4"/>
     </row>
-    <row r="525" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="525" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D525" s="4"/>
     </row>
-    <row r="526" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="526" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D526" s="4"/>
     </row>
-    <row r="527" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="527" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D527" s="4"/>
     </row>
-    <row r="528" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="528" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D528" s="4"/>
     </row>
+    <row r="529" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D529" s="4"/>
+    </row>
+    <row r="530" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D530" s="4"/>
+    </row>
+    <row r="531" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D531" s="4"/>
+    </row>
+    <row r="532" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D532" s="4"/>
+    </row>
+    <row r="533" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D533" s="4"/>
+    </row>
+    <row r="534" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D534" s="4"/>
+    </row>
+    <row r="535" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D535" s="4"/>
+    </row>
+    <row r="536" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D536" s="4"/>
+    </row>
+    <row r="537" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D537" s="4"/>
+    </row>
+    <row r="538" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D538" s="4"/>
+    </row>
+    <row r="539" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D539" s="4"/>
+    </row>
+    <row r="540" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D540" s="4"/>
+    </row>
+    <row r="541" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D541" s="4"/>
+    </row>
+    <row r="542" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D542" s="4"/>
+    </row>
+    <row r="543" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D543" s="4"/>
+    </row>
+    <row r="544" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D544" s="4"/>
+    </row>
+    <row r="545" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D545" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="B18:B25"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B33:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="B57:B62"/>
+  <mergeCells count="15">
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C79:C82"/>
+    <mergeCell ref="B69:B82"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B3:B22"/>
+    <mergeCell ref="B25:B32"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1" display="IBEX" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E23" r:id="rId1" display="IBEX" xr:uid="{702014FC-EDB2-4E19-A7B3-E423EF272C7E}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -3412,7 +3860,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>D3:D528</xm:sqref>
+          <xm:sqref>D3:D545</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3428,52 +3876,52 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>

</xml_diff>